<commit_message>
switching to a new sheet and populating it
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -457,14 +457,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>First name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Last name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
writing in a loop
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="business basic info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="This_is_sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="test_data1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -480,4 +481,37 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>keys</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Creating simple table from simple dict
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -10,6 +10,7 @@
     <sheet name="business basic info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="This_is_sheet2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="test_data1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="test_data2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -514,4 +515,71 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="C5:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>key1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>value1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>key2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>value2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>key3</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>value3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding a title to example table
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -523,7 +523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C5:D8"/>
+  <dimension ref="C4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>This is test1 table</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
wip - new table data
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -11,6 +11,7 @@
     <sheet name="This_is_sheet2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="test_data1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="test_data2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="test_data3" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -589,4 +590,78 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="C14:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Sweden_Pay_Now_Direct_debit</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>column_name1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>value1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>column_name2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>value2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>column_name3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>value3</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>column_name4</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
exporting data from 2 tables + fixup
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -598,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C14:D18"/>
+  <dimension ref="B14:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,55 +607,103 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="14">
-      <c r="C14" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>Sweden_Pay_Now_Direct_debit</t>
         </is>
       </c>
     </row>
     <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>column_name1</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>value1</t>
+          <t>value4</t>
         </is>
       </c>
     </row>
     <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>column_name2</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>value2</t>
+          <t>value4</t>
         </is>
       </c>
     </row>
     <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>column_name3</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>value3</t>
+          <t>value4</t>
         </is>
       </c>
     </row>
     <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sweden_Pay_Now_Card</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>column_name4</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>value4</t>
         </is>

</xml_diff>

<commit_message>
fixup, adding space between tables
</commit_message>
<xml_diff>
--- a/fist_example.xlsx
+++ b/fist_example.xlsx
@@ -598,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B14:C22"/>
+  <dimension ref="B16:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,34 +606,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Sweden_Pay_Now_Direct_debit</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>key4</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>value4</t>
-        </is>
-      </c>
-    </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>key4</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>value4</t>
+          <t>Sweden_Pay_Now_Direct_debit</t>
         </is>
       </c>
     </row>
@@ -652,7 +628,7 @@
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sweden_Pay_Now_Card</t>
+          <t>key4</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -685,25 +661,56 @@
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>key4</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>value4</t>
-        </is>
-      </c>
-    </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>key4</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
+          <t>Sweden_Pay_Now_Card</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>value4</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>key4</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>value4</t>
         </is>

</xml_diff>